<commit_message>
Recruitment Settings Pages API calls
</commit_message>
<xml_diff>
--- a/attendance/src/main/resources/Sanity.xlsx
+++ b/attendance/src/main/resources/Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mouni\IdeaProjects\Master\Automation_Project\attendance\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61EC955D-21E5-448E-A5EA-C77AB4D6B0AF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4A6CED-B3F1-469F-B5A5-53D450D9CDBE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="251">
   <si>
     <t>TCID</t>
   </si>
@@ -783,15 +783,6 @@
   </si>
   <si>
     <t>25,26,27,28</t>
-  </si>
-  <si>
-    <t>75</t>
-  </si>
-  <si>
-    <t>Recruitment</t>
-  </si>
-  <si>
-    <t>com.darwinbox.attendance.shifts.CRUDOperations</t>
   </si>
 </sst>
 </file>
@@ -1163,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76:H76"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76:C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3129,27 +3120,9 @@
       </c>
     </row>
     <row r="76" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="E76" t="s">
-        <v>253</v>
-      </c>
-      <c r="F76" t="s">
-        <v>158</v>
-      </c>
-      <c r="G76" t="s">
-        <v>159</v>
-      </c>
-      <c r="H76" t="s">
-        <v>9</v>
-      </c>
+      <c r="A76" s="4"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
     </row>
     <row r="77" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>

</xml_diff>